<commit_message>
Button gameOver Tapout Broadcast
</commit_message>
<xml_diff>
--- a/Drivers Ready Button Communication Matrix.xlsx
+++ b/Drivers Ready Button Communication Matrix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\kurti\Git\Drivers-Ready-Buttons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E8C886DE-B9FC-4CB8-9653-1FF1E099423F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F7BF1B2-7A7F-4E43-B85E-B90F9E1B8F9A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="8370" activeTab="1" xr2:uid="{60700B47-1243-4D70-9110-CC239BDFAD13}"/>
+    <workbookView xWindow="1260" yWindow="4170" windowWidth="21600" windowHeight="11835" activeTab="1" xr2:uid="{60700B47-1243-4D70-9110-CC239BDFAD13}"/>
   </bookViews>
   <sheets>
     <sheet name="Communication Matrix" sheetId="1" r:id="rId1"/>
@@ -148,9 +148,6 @@
     <t>Used to signal last 30 seconds, and current time on clock, to all buttons</t>
   </si>
   <si>
-    <t>Used to signal gameOver to buttons, or to signal a team tapout</t>
-  </si>
-  <si>
     <t>Used to command buttons to non-lighted status</t>
   </si>
   <si>
@@ -170,6 +167,9 @@
   </si>
   <si>
     <t>Sent by Base to 'Arm' Button for match begin</t>
+  </si>
+  <si>
+    <t>Used to signal gameOver to buttons, or to signal a team tapout. Data is initiator ID</t>
   </si>
 </sst>
 </file>
@@ -185,12 +185,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -205,7 +211,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -213,8 +219,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -534,7 +546,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -543,27 +555,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="3"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="2"/>
+      <c r="E1" s="3"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -572,144 +578,144 @@
       <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E3" s="4"/>
+      <c r="D3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
+      <c r="A4" s="3"/>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
       <c r="C4" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2"/>
+      <c r="A5" s="3"/>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
       <c r="C5" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="4"/>
+      <c r="D5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="3"/>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="4"/>
+      <c r="D6" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2"/>
+      <c r="A7" s="3"/>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="C7" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="4"/>
+      <c r="D7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2"/>
+      <c r="A8" s="3"/>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C8" t="s">
         <v>23</v>
       </c>
-      <c r="D8" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="4" t="s">
+      <c r="D8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2"/>
+      <c r="A9" s="3"/>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
       <c r="C9" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="4"/>
+      <c r="D9" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2"/>
+      <c r="A10" s="3"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="C10" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4" t="s">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2"/>
+      <c r="A11" s="3"/>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="C11" t="s">
         <v>26</v>
       </c>
-      <c r="D11" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="4"/>
+      <c r="D11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2"/>
-      <c r="B12" s="1" t="s">
+      <c r="A12" s="3"/>
+      <c r="B12" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E12" s="4" t="s">
+      <c r="D12" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E12" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2"/>
+      <c r="A13" s="3"/>
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>
       <c r="C13" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="E13" s="4"/>
+      <c r="D13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -725,19 +731,19 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="4"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
     <col min="2" max="2" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9.140625" style="1"/>
-    <col min="5" max="5" width="68.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="74.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B1" t="s">
@@ -754,7 +760,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B2" t="s">
@@ -771,7 +777,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
@@ -788,7 +794,7 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
@@ -805,7 +811,7 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B5" t="s">
@@ -822,7 +828,7 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B6" t="s">
@@ -839,7 +845,7 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B7" t="s">
@@ -852,11 +858,11 @@
         <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>38</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B8" t="s">
@@ -869,11 +875,11 @@
         <v>32</v>
       </c>
       <c r="E8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="4" t="s">
+      <c r="A9" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B9" t="s">
@@ -883,14 +889,14 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
+        <v>39</v>
+      </c>
+      <c r="E9" t="s">
         <v>40</v>
       </c>
-      <c r="E9" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="4" t="s">
+      <c r="A10" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B10" t="s">
@@ -903,11 +909,11 @@
         <v>32</v>
       </c>
       <c r="E10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B11" t="s">
@@ -917,14 +923,14 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
+        <v>42</v>
+      </c>
+      <c r="E11" t="s">
         <v>43</v>
       </c>
-      <c r="E11" t="s">
-        <v>44</v>
-      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="4" t="s">
+      <c r="A12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B12" t="s">
@@ -937,7 +943,7 @@
         <v>32</v>
       </c>
       <c r="E12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Now with more switch statements
</commit_message>
<xml_diff>
--- a/Drivers Ready Button Communication Matrix.xlsx
+++ b/Drivers Ready Button Communication Matrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\kurti\Git\Drivers-Ready-Buttons\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F7E6AF9-C1AC-4135-B86D-F50AE1B26382}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BABCEBD-5834-40B9-B08F-B125F374288E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1260" yWindow="4170" windowWidth="21600" windowHeight="11835" xr2:uid="{60700B47-1243-4D70-9110-CC239BDFAD13}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="46">
   <si>
     <t>PG</t>
   </si>
@@ -232,10 +232,10 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -555,7 +555,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -564,10 +564,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="6"/>
+      <c r="E1" s="7"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="D2" s="2" t="s">
@@ -578,7 +578,7 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -587,13 +587,13 @@
       <c r="C3" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="6" t="s">
         <v>29</v>
       </c>
       <c r="E3" s="2"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
+      <c r="A4" s="7"/>
       <c r="B4" s="1" t="s">
         <v>5</v>
       </c>
@@ -601,12 +601,12 @@
         <v>19</v>
       </c>
       <c r="D4" s="2"/>
-      <c r="E4" s="7" t="s">
+      <c r="E4" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
+      <c r="A5" s="7"/>
       <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
@@ -619,7 +619,7 @@
       <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6"/>
+      <c r="A6" s="7"/>
       <c r="B6" s="1" t="s">
         <v>7</v>
       </c>
@@ -632,7 +632,7 @@
       <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6"/>
+      <c r="A7" s="7"/>
       <c r="B7" s="1" t="s">
         <v>8</v>
       </c>
@@ -645,7 +645,7 @@
       <c r="E7" s="2"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="6"/>
+      <c r="A8" s="7"/>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
@@ -655,12 +655,12 @@
       <c r="D8" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="7" t="s">
+      <c r="E8" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="6"/>
+      <c r="A9" s="7"/>
       <c r="B9" s="1" t="s">
         <v>10</v>
       </c>
@@ -673,7 +673,7 @@
       <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="6"/>
+      <c r="A10" s="7"/>
       <c r="B10" s="1" t="s">
         <v>11</v>
       </c>
@@ -681,12 +681,12 @@
         <v>25</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="7" t="s">
+      <c r="E10" s="6" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="1" t="s">
         <v>12</v>
       </c>
@@ -699,7 +699,7 @@
       <c r="E11" s="2"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="6"/>
+      <c r="A12" s="7"/>
       <c r="B12" s="3" t="s">
         <v>13</v>
       </c>
@@ -714,7 +714,7 @@
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="6"/>
+      <c r="A13" s="7"/>
       <c r="B13" s="1" t="s">
         <v>14</v>
       </c>

</xml_diff>